<commit_message>
Fixed data dictionary for users
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\the-b\Desktop\SE\github\SE_Gruppo10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED85B8C7-FFB3-446B-850E-34ADBC7FD422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B915530-C4BE-49A1-85F4-AD6336DF33A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1453B895-971B-48B0-A747-19F56A6574F3}"/>
+    <workbookView xWindow="5790" yWindow="2775" windowWidth="28800" windowHeight="15435" xr2:uid="{1453B895-971B-48B0-A747-19F56A6574F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>Data Type</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -105,7 +102,10 @@
     <t>planner</t>
   </si>
   <si>
-    <t>Data Dictionary</t>
+    <t>users</t>
+  </si>
+  <si>
+    <t>Data Dictionary for users</t>
   </si>
 </sst>
 </file>
@@ -217,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -231,18 +231,21 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -258,7 +261,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -557,27 +560,33 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" customWidth="1"/>
-    <col min="4" max="4" width="25.6328125" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" customWidth="1"/>
-    <col min="7" max="7" width="28.81640625" customWidth="1"/>
-    <col min="8" max="8" width="66.1796875" customWidth="1"/>
+    <col min="1" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1"/>
+    <col min="8" max="8" width="66.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,79 +612,80 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="131" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="5"/>
-      <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="6" spans="1:8" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>